<commit_message>
I went through the logic of the SUMIFS drill from Chandoo
</commit_message>
<xml_diff>
--- a/Interesting_SUMIFS_Use_From_Chandoo.xlsx
+++ b/Interesting_SUMIFS_Use_From_Chandoo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{53AC8EE3-5D3D-4588-A3B2-AD621DE6D2E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDFAD33B-0D46-4CDC-B788-AC3E79567EDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="225" windowWidth="25440" windowHeight="15270" xr2:uid="{26D4546B-D2A1-4444-8EAF-A6228F96F0C1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{26D4546B-D2A1-4444-8EAF-A6228F96F0C1}"/>
   </bookViews>
   <sheets>
     <sheet name="IF IF IF IF IF" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -584,7 +584,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -670,6 +670,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -756,151 +757,180 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>155864</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>25977</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>225136</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>178375</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>1402772</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>25977</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>467589</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>178376</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Rectangle: Rounded Corners 1">
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="5" name="Group 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E5E062C-4777-FA9F-7E4B-3AF454DC03D6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6785DAB-94F0-8EF7-764F-9E736EC7E867}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="8096250" y="1073727"/>
-          <a:ext cx="3273136" cy="1524000"/>
+          <a:off x="13102936" y="1563830"/>
+          <a:ext cx="3290453" cy="1440873"/>
+          <a:chOff x="8323118" y="1113558"/>
+          <a:chExt cx="3290453" cy="1440873"/>
         </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst>
-            <a:gd name="adj" fmla="val 7108"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1">
-            <a:lumMod val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="2" name="Rectangle: Rounded Corners 1">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E5E062C-4777-FA9F-7E4B-3AF454DC03D6}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8323118" y="1113558"/>
+            <a:ext cx="3290453" cy="1440873"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 7108"/>
+            </a:avLst>
+          </a:prstGeom>
           <a:solidFill>
             <a:schemeClr val="bg1">
-              <a:lumMod val="75000"/>
+              <a:lumMod val="95000"/>
             </a:schemeClr>
           </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="85000"/>
-                  <a:lumOff val="15000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Learn more about this technique:</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>305666</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>60614</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>1154257</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>112568</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Rectangle: Rounded Corners 2">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3ADB4FC4-0966-0F66-A942-3EB894941D21}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8453871" y="1489364"/>
-          <a:ext cx="2667000" cy="432954"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="tx1">
-              <a:lumMod val="75000"/>
-              <a:lumOff val="25000"/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
             </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent4"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent4"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent4"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="1">
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Learn more about this technique:</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="3" name="Rectangle: Rounded Corners 2">
+            <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3ADB4FC4-0966-0F66-A942-3EB894941D21}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8673811" y="1446069"/>
+            <a:ext cx="2677391" cy="412172"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent4"/>
+          </a:lnRef>
+          <a:fillRef idx="3">
+            <a:schemeClr val="accent4"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="accent4"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+              </a:rPr>
+              <a:t>Read the article </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-NZ" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+              </a:rPr>
+              <a:t>📰</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1200" b="1">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="85000"/>
@@ -909,11 +939,85 @@
               </a:solidFill>
               <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
               <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
-            </a:rPr>
-            <a:t>Read the article </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-NZ" sz="1200" b="1">
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="6" name="Rectangle: Rounded Corners 5">
+            <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA0C924A-32A7-E4C5-0157-065F91FA83DE}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8673811" y="1956955"/>
+            <a:ext cx="2677391" cy="412172"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent5"/>
+          </a:lnRef>
+          <a:fillRef idx="3">
+            <a:schemeClr val="accent5"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="accent5"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+              </a:rPr>
+              <a:t>Watch the video </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-NZ" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+                <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+              </a:rPr>
+              <a:t>📺</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1200" b="1">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="85000"/>
@@ -922,124 +1026,11 @@
               </a:solidFill>
               <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
               <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
-            </a:rPr>
-            <a:t>📰</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1200" b="1">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="85000"/>
-                <a:lumOff val="15000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
-            <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>305666</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>31173</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>1154257</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>83127</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Rectangle: Rounded Corners 5">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA0C924A-32A7-E4C5-0157-065F91FA83DE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8453871" y="2031423"/>
-          <a:ext cx="2667000" cy="432954"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="tx1">
-              <a:lumMod val="75000"/>
-              <a:lumOff val="25000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent5"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="1">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="85000"/>
-                  <a:lumOff val="15000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
-              <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
-            </a:rPr>
-            <a:t>Watch the video </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-NZ" sz="1200" b="1">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="85000"/>
-                  <a:lumOff val="15000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
-              <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
-            </a:rPr>
-            <a:t>📺</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1200" b="1">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="85000"/>
-                <a:lumOff val="15000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
-            <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1369,7 +1360,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="595" row="10">
+  <wetp:taskpane dockstate="right" visibility="0" width="757" row="7">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1384,6 +1375,13 @@
   <we:properties/>
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
 </we:webextension>
 </file>
 
@@ -1394,34 +1392,34 @@
   </sheetPr>
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5:K44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" customWidth="1"/>
-    <col min="2" max="2" width="3.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="1.6640625" customWidth="1"/>
+    <col min="2" max="2" width="3.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" customWidth="1"/>
-    <col min="11" max="11" width="3.140625" customWidth="1"/>
-    <col min="15" max="15" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" customWidth="1"/>
+    <col min="11" max="11" width="11.44140625" customWidth="1"/>
+    <col min="15" max="15" width="21.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="2" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="C1" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D1" s="3"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H3" s="16" t="s">
         <v>95</v>
       </c>
@@ -1429,7 +1427,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C4" s="7" t="s">
         <v>25</v>
       </c>
@@ -1452,7 +1450,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C5" s="18" t="s">
         <v>55</v>
       </c>
@@ -1483,8 +1481,23 @@
 discount[Quantity from],"&lt;="&amp;G5, discount[Quantity to],"&gt;="&amp;G5))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K5" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F5, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D5 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E5 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G5,
+        discount[Quantity to], "&gt;=" &amp; G5
+    )
+)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C6" s="20" t="s">
         <v>56</v>
       </c>
@@ -1515,8 +1528,23 @@
 discount[Quantity from],"&lt;="&amp;G6, discount[Quantity to],"&gt;="&amp;G6))</f>
         <v>0.04</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K6" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F6, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D6 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E6 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G6,
+        discount[Quantity to], "&gt;=" &amp; G6
+    )
+)</f>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C7" s="19" t="s">
         <v>57</v>
       </c>
@@ -1547,8 +1575,23 @@
 discount[Quantity from],"&lt;="&amp;G7, discount[Quantity to],"&gt;="&amp;G7))</f>
         <v>0.05</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K7" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F7, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D7 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E7 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G7,
+        discount[Quantity to], "&gt;=" &amp; G7
+    )
+)</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C8" s="20" t="s">
         <v>58</v>
       </c>
@@ -1579,8 +1622,23 @@
 discount[Quantity from],"&lt;="&amp;G8, discount[Quantity to],"&gt;="&amp;G8))</f>
         <v>0.06</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K8" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F8, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D8 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E8 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G8,
+        discount[Quantity to], "&gt;=" &amp; G8
+    )
+)</f>
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C9" s="19" t="s">
         <v>59</v>
       </c>
@@ -1611,8 +1669,23 @@
 discount[Quantity from],"&lt;="&amp;G9, discount[Quantity to],"&gt;="&amp;G9))</f>
         <v>0.06</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K9" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F9, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D9 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E9 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G9,
+        discount[Quantity to], "&gt;=" &amp; G9
+    )
+)</f>
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C10" s="20" t="s">
         <v>60</v>
       </c>
@@ -1643,8 +1716,23 @@
 discount[Quantity from],"&lt;="&amp;G10, discount[Quantity to],"&gt;="&amp;G10))</f>
         <v>3.5000000000000003E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K10" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F10, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D10 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E10 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G10,
+        discount[Quantity to], "&gt;=" &amp; G10
+    )
+)</f>
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C11" s="19" t="s">
         <v>61</v>
       </c>
@@ -1675,8 +1763,23 @@
 discount[Quantity from],"&lt;="&amp;G11, discount[Quantity to],"&gt;="&amp;G11))</f>
         <v>0.05</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K11" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F11, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D11 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E11 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G11,
+        discount[Quantity to], "&gt;=" &amp; G11
+    )
+)</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C12" s="20" t="s">
         <v>62</v>
       </c>
@@ -1707,8 +1810,23 @@
 discount[Quantity from],"&lt;="&amp;G12, discount[Quantity to],"&gt;="&amp;G12))</f>
         <v>0.05</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K12" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F12, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D12 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E12 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G12,
+        discount[Quantity to], "&gt;=" &amp; G12
+    )
+)</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C13" s="19" t="s">
         <v>63</v>
       </c>
@@ -1732,8 +1850,23 @@
 discount[Quantity from],"&lt;="&amp;G13, discount[Quantity to],"&gt;="&amp;G13))</f>
         <v>0.03</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K13" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F13, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D13 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E13 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G13,
+        discount[Quantity to], "&gt;=" &amp; G13
+    )
+)</f>
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C14" s="20" t="s">
         <v>64</v>
       </c>
@@ -1757,8 +1890,23 @@
 discount[Quantity from],"&lt;="&amp;G14, discount[Quantity to],"&gt;="&amp;G14))</f>
         <v>0.08</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K14" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F14, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D14 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E14 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G14,
+        discount[Quantity to], "&gt;=" &amp; G14
+    )
+)</f>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C15" s="19" t="s">
         <v>65</v>
       </c>
@@ -1782,9 +1930,24 @@
 discount[Quantity from],"&lt;="&amp;G15, discount[Quantity to],"&gt;="&amp;G15))</f>
         <v>0.05</v>
       </c>
+      <c r="K15" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F15, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D15 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E15 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G15,
+        discount[Quantity to], "&gt;=" &amp; G15
+    )
+)</f>
+        <v>0.05</v>
+      </c>
       <c r="M15" s="41"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C16" s="20" t="s">
         <v>66</v>
       </c>
@@ -1808,9 +1971,24 @@
 discount[Quantity from],"&lt;="&amp;G16, discount[Quantity to],"&gt;="&amp;G16))</f>
         <v>4.4999999999999998E-2</v>
       </c>
+      <c r="K16" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F16, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D16 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E16 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G16,
+        discount[Quantity to], "&gt;=" &amp; G16
+    )
+)</f>
+        <v>4.4999999999999998E-2</v>
+      </c>
       <c r="M16" s="42"/>
     </row>
-    <row r="17" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C17" s="19" t="s">
         <v>67</v>
       </c>
@@ -1834,9 +2012,24 @@
 discount[Quantity from],"&lt;="&amp;G17, discount[Quantity to],"&gt;="&amp;G17))</f>
         <v>3.5000000000000003E-2</v>
       </c>
+      <c r="K17" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F17, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D17 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E17 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G17,
+        discount[Quantity to], "&gt;=" &amp; G17
+    )
+)</f>
+        <v>3.5000000000000003E-2</v>
+      </c>
       <c r="M17" s="42"/>
     </row>
-    <row r="18" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C18" s="20" t="s">
         <v>68</v>
       </c>
@@ -1860,9 +2053,24 @@
 discount[Quantity from],"&lt;="&amp;G18, discount[Quantity to],"&gt;="&amp;G18))</f>
         <v>3.5000000000000003E-2</v>
       </c>
+      <c r="K18" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F18, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D18 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E18 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G18,
+        discount[Quantity to], "&gt;=" &amp; G18
+    )
+)</f>
+        <v>3.5000000000000003E-2</v>
+      </c>
       <c r="M18" s="42"/>
     </row>
-    <row r="19" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C19" s="19" t="s">
         <v>69</v>
       </c>
@@ -1886,9 +2094,24 @@
 discount[Quantity from],"&lt;="&amp;G19, discount[Quantity to],"&gt;="&amp;G19))</f>
         <v>0.05</v>
       </c>
+      <c r="K19" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F19, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D19 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E19 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G19,
+        discount[Quantity to], "&gt;=" &amp; G19
+    )
+)</f>
+        <v>0.05</v>
+      </c>
       <c r="M19" s="42"/>
     </row>
-    <row r="20" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C20" s="20" t="s">
         <v>70</v>
       </c>
@@ -1912,8 +2135,23 @@
 discount[Quantity from],"&lt;="&amp;G20, discount[Quantity to],"&gt;="&amp;G20))</f>
         <v>0.04</v>
       </c>
-    </row>
-    <row r="21" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="K20" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F20, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D20 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E20 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G20,
+        discount[Quantity to], "&gt;=" &amp; G20
+    )
+)</f>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C21" s="19" t="s">
         <v>71</v>
       </c>
@@ -1937,8 +2175,23 @@
 discount[Quantity from],"&lt;="&amp;G21, discount[Quantity to],"&gt;="&amp;G21))</f>
         <v>0.03</v>
       </c>
-    </row>
-    <row r="22" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="K21" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F21, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D21 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E21 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G21,
+        discount[Quantity to], "&gt;=" &amp; G21
+    )
+)</f>
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C22" s="20" t="s">
         <v>72</v>
       </c>
@@ -1962,8 +2215,23 @@
 discount[Quantity from],"&lt;="&amp;G22, discount[Quantity to],"&gt;="&amp;G22))</f>
         <v>0.05</v>
       </c>
-    </row>
-    <row r="23" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="K22" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F22, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D22 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E22 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G22,
+        discount[Quantity to], "&gt;=" &amp; G22
+    )
+)</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C23" s="19" t="s">
         <v>73</v>
       </c>
@@ -1987,8 +2255,23 @@
 discount[Quantity from],"&lt;="&amp;G23, discount[Quantity to],"&gt;="&amp;G23))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="K23" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F23, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D23 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E23 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G23,
+        discount[Quantity to], "&gt;=" &amp; G23
+    )
+)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C24" s="20" t="s">
         <v>74</v>
       </c>
@@ -2012,8 +2295,23 @@
 discount[Quantity from],"&lt;="&amp;G24, discount[Quantity to],"&gt;="&amp;G24))</f>
         <v>0.04</v>
       </c>
-    </row>
-    <row r="25" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="K24" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F24, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D24 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E24 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G24,
+        discount[Quantity to], "&gt;=" &amp; G24
+    )
+)</f>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="25" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C25" s="19" t="s">
         <v>55</v>
       </c>
@@ -2037,8 +2335,23 @@
 discount[Quantity from],"&lt;="&amp;G25, discount[Quantity to],"&gt;="&amp;G25))</f>
         <v>0.03</v>
       </c>
-    </row>
-    <row r="26" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="K25" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F25, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D25 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E25 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G25,
+        discount[Quantity to], "&gt;=" &amp; G25
+    )
+)</f>
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="26" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C26" s="20" t="s">
         <v>56</v>
       </c>
@@ -2062,8 +2375,23 @@
 discount[Quantity from],"&lt;="&amp;G26, discount[Quantity to],"&gt;="&amp;G26))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="K26" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F26, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D26 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E26 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G26,
+        discount[Quantity to], "&gt;=" &amp; G26
+    )
+)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C27" s="19" t="s">
         <v>57</v>
       </c>
@@ -2087,8 +2415,23 @@
 discount[Quantity from],"&lt;="&amp;G27, discount[Quantity to],"&gt;="&amp;G27))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="K27" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F27, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D27 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E27 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G27,
+        discount[Quantity to], "&gt;=" &amp; G27
+    )
+)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C28" s="20" t="s">
         <v>58</v>
       </c>
@@ -2112,8 +2455,23 @@
 discount[Quantity from],"&lt;="&amp;G28, discount[Quantity to],"&gt;="&amp;G28))</f>
         <v>0.04</v>
       </c>
-    </row>
-    <row r="29" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="K28" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F28, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D28 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E28 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G28,
+        discount[Quantity to], "&gt;=" &amp; G28
+    )
+)</f>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="29" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C29" s="19" t="s">
         <v>59</v>
       </c>
@@ -2137,8 +2495,23 @@
 discount[Quantity from],"&lt;="&amp;G29, discount[Quantity to],"&gt;="&amp;G29))</f>
         <v>0.05</v>
       </c>
-    </row>
-    <row r="30" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="K29" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F29, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D29 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E29 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G29,
+        discount[Quantity to], "&gt;=" &amp; G29
+    )
+)</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="30" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C30" s="20" t="s">
         <v>60</v>
       </c>
@@ -2162,8 +2535,23 @@
 discount[Quantity from],"&lt;="&amp;G30, discount[Quantity to],"&gt;="&amp;G30))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="K30" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F30, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D30 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E30 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G30,
+        discount[Quantity to], "&gt;=" &amp; G30
+    )
+)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C31" s="19" t="s">
         <v>61</v>
       </c>
@@ -2187,8 +2575,23 @@
 discount[Quantity from],"&lt;="&amp;G31, discount[Quantity to],"&gt;="&amp;G31))</f>
         <v>0.04</v>
       </c>
-    </row>
-    <row r="32" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="K31" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F31, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D31 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E31 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G31,
+        discount[Quantity to], "&gt;=" &amp; G31
+    )
+)</f>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="32" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C32" s="20" t="s">
         <v>62</v>
       </c>
@@ -2212,8 +2615,23 @@
 discount[Quantity from],"&lt;="&amp;G32, discount[Quantity to],"&gt;="&amp;G32))</f>
         <v>4.4999999999999998E-2</v>
       </c>
-    </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K32" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F32, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D32 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E32 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G32,
+        discount[Quantity to], "&gt;=" &amp; G32
+    )
+)</f>
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C33" s="19" t="s">
         <v>63</v>
       </c>
@@ -2237,8 +2655,23 @@
 discount[Quantity from],"&lt;="&amp;G33, discount[Quantity to],"&gt;="&amp;G33))</f>
         <v>0.05</v>
       </c>
-    </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K33" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F33, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D33 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E33 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G33,
+        discount[Quantity to], "&gt;=" &amp; G33
+    )
+)</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="34" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C34" s="20" t="s">
         <v>64</v>
       </c>
@@ -2262,8 +2695,23 @@
 discount[Quantity from],"&lt;="&amp;G34, discount[Quantity to],"&gt;="&amp;G34))</f>
         <v>3.5000000000000003E-2</v>
       </c>
-    </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K34" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F34, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D34 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E34 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G34,
+        discount[Quantity to], "&gt;=" &amp; G34
+    )
+)</f>
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C35" s="19" t="s">
         <v>65</v>
       </c>
@@ -2287,8 +2735,23 @@
 discount[Quantity from],"&lt;="&amp;G35, discount[Quantity to],"&gt;="&amp;G35))</f>
         <v>0.03</v>
       </c>
-    </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K35" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F35, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D35 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E35 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G35,
+        discount[Quantity to], "&gt;=" &amp; G35
+    )
+)</f>
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="36" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C36" s="20" t="s">
         <v>66</v>
       </c>
@@ -2312,8 +2775,23 @@
 discount[Quantity from],"&lt;="&amp;G36, discount[Quantity to],"&gt;="&amp;G36))</f>
         <v>0.04</v>
       </c>
-    </row>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K36" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F36, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D36 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E36 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G36,
+        discount[Quantity to], "&gt;=" &amp; G36
+    )
+)</f>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="37" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C37" s="19" t="s">
         <v>67</v>
       </c>
@@ -2337,8 +2815,23 @@
 discount[Quantity from],"&lt;="&amp;G37, discount[Quantity to],"&gt;="&amp;G37))</f>
         <v>3.5000000000000003E-2</v>
       </c>
-    </row>
-    <row r="38" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K37" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F37, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D37 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E37 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G37,
+        discount[Quantity to], "&gt;=" &amp; G37
+    )
+)</f>
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C38" s="20" t="s">
         <v>68</v>
       </c>
@@ -2362,8 +2855,23 @@
 discount[Quantity from],"&lt;="&amp;G38, discount[Quantity to],"&gt;="&amp;G38))</f>
         <v>0.05</v>
       </c>
-    </row>
-    <row r="39" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K38" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F38, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D38 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E38 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G38,
+        discount[Quantity to], "&gt;=" &amp; G38
+    )
+)</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="39" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C39" s="19" t="s">
         <v>69</v>
       </c>
@@ -2387,8 +2895,23 @@
 discount[Quantity from],"&lt;="&amp;G39, discount[Quantity to],"&gt;="&amp;G39))</f>
         <v>0.04</v>
       </c>
-    </row>
-    <row r="40" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K39" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F39, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D39 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E39 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G39,
+        discount[Quantity to], "&gt;=" &amp; G39
+    )
+)</f>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="40" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C40" s="20" t="s">
         <v>70</v>
       </c>
@@ -2412,8 +2935,23 @@
 discount[Quantity from],"&lt;="&amp;G40, discount[Quantity to],"&gt;="&amp;G40))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K40" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F40, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D40 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E40 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G40,
+        discount[Quantity to], "&gt;=" &amp; G40
+    )
+)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C41" s="19" t="s">
         <v>71</v>
       </c>
@@ -2437,8 +2975,23 @@
 discount[Quantity from],"&lt;="&amp;G41, discount[Quantity to],"&gt;="&amp;G41))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K41" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F41, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D41 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E41 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G41,
+        discount[Quantity to], "&gt;=" &amp; G41
+    )
+)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C42" s="20" t="s">
         <v>72</v>
       </c>
@@ -2462,8 +3015,23 @@
 discount[Quantity from],"&lt;="&amp;G42, discount[Quantity to],"&gt;="&amp;G42))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K42" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F42, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D42 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E42 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G42,
+        discount[Quantity to], "&gt;=" &amp; G42
+    )
+)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C43" s="19" t="s">
         <v>73</v>
       </c>
@@ -2487,8 +3055,23 @@
 discount[Quantity from],"&lt;="&amp;G43, discount[Quantity to],"&gt;="&amp;G43))</f>
         <v>0.03</v>
       </c>
-    </row>
-    <row r="44" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K43" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F43, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D43 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E43 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G43,
+        discount[Quantity to], "&gt;=" &amp; G43
+    )
+)</f>
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="44" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C44" s="20" t="s">
         <v>74</v>
       </c>
@@ -2510,6 +3093,21 @@
 SUMIFS(discount[Discount], discount[Country],"*"&amp;D44&amp;"*",
 discount[Category],_xlpm.cat, discount[Customer Type],"*"&amp;E44&amp;"*",
 discount[Quantity from],"&lt;="&amp;G44, discount[Quantity to],"&gt;="&amp;G44))</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="K44" s="43">
+        <f>_xlfn.LET(
+    _xlpm.cat, "*" &amp; _xlfn.XLOOKUP(F44, products[Name], products[Category]) &amp;
+        "*",
+    SUMIFS(
+        discount[Discount],
+        discount[Country], "*" &amp; D44 &amp; "*",
+        discount[Category], _xlpm.cat,
+        discount[Customer Type], "*" &amp; E44 &amp; "*",
+        discount[Quantity from], "&lt;=" &amp; G44,
+        discount[Quantity to], "&gt;=" &amp; G44
+    )
+)</f>
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -2534,26 +3132,26 @@
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="4" width="2" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" customWidth="1"/>
-    <col min="8" max="8" width="4.85546875" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" customWidth="1"/>
-    <col min="10" max="10" width="4.5703125" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" customWidth="1"/>
-    <col min="14" max="14" width="4.85546875" customWidth="1"/>
-    <col min="15" max="15" width="5.42578125" customWidth="1"/>
-    <col min="16" max="16" width="4.5703125" customWidth="1"/>
-    <col min="17" max="17" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="23.5546875" customWidth="1"/>
+    <col min="8" max="8" width="4.88671875" customWidth="1"/>
+    <col min="9" max="9" width="5.44140625" customWidth="1"/>
+    <col min="10" max="10" width="4.5546875" customWidth="1"/>
+    <col min="11" max="11" width="19.109375" customWidth="1"/>
+    <col min="14" max="14" width="4.88671875" customWidth="1"/>
+    <col min="15" max="15" width="5.44140625" customWidth="1"/>
+    <col min="16" max="16" width="4.5546875" customWidth="1"/>
+    <col min="17" max="17" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
         <v>2</v>
       </c>
@@ -2576,7 +3174,7 @@
       <c r="Q4" s="9"/>
       <c r="R4" s="10"/>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5" s="11"/>
       <c r="C5" s="32" t="s">
         <v>3</v>
@@ -2595,7 +3193,7 @@
       </c>
       <c r="R5" s="12"/>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B6" s="11"/>
       <c r="D6" s="32" t="s">
         <v>4</v>
@@ -2615,7 +3213,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B7" s="11"/>
       <c r="E7" s="32" t="s">
         <v>5</v>
@@ -2638,7 +3236,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8" s="11"/>
       <c r="E8" s="34" t="s">
         <v>6</v>
@@ -2661,7 +3259,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" s="11"/>
       <c r="C9" s="32" t="s">
         <v>97</v>
@@ -2680,7 +3278,7 @@
       </c>
       <c r="R9" s="12"/>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B10" s="11"/>
       <c r="D10" s="32" t="s">
         <v>7</v>
@@ -2700,7 +3298,7 @@
       </c>
       <c r="R10" s="12"/>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B11" s="11"/>
       <c r="E11" s="32" t="s">
         <v>5</v>
@@ -2721,7 +3319,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B12" s="11"/>
       <c r="E12" s="34" t="s">
         <v>6</v>
@@ -2744,7 +3342,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B13" s="11"/>
       <c r="D13" s="32" t="s">
         <v>8</v>
@@ -2764,7 +3362,7 @@
       </c>
       <c r="R13" s="12"/>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B14" s="11"/>
       <c r="E14" s="32" t="s">
         <v>9</v>
@@ -2789,7 +3387,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B15" s="11"/>
       <c r="C15" s="32" t="s">
         <v>98</v>
@@ -2803,7 +3401,7 @@
       </c>
       <c r="R15" s="12"/>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B16" s="11"/>
       <c r="D16" s="32" t="s">
         <v>12</v>
@@ -2822,7 +3420,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="11"/>
       <c r="D17" s="34" t="s">
         <v>13</v>
@@ -2832,7 +3430,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="13"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6" t="s">
@@ -2843,10 +3441,10 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F19" s="5"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F31" s="5"/>
     </row>
   </sheetData>
@@ -2865,16 +3463,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" customWidth="1"/>
     <col min="3" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>83</v>
       </c>
@@ -2894,7 +3492,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>90</v>
       </c>
@@ -2914,7 +3512,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>90</v>
       </c>
@@ -2934,7 +3532,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>90</v>
       </c>
@@ -2954,7 +3552,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>90</v>
       </c>
@@ -2974,7 +3572,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>90</v>
       </c>
@@ -2994,7 +3592,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>90</v>
       </c>
@@ -3014,7 +3612,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>90</v>
       </c>
@@ -3034,7 +3632,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>90</v>
       </c>
@@ -3054,7 +3652,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>91</v>
       </c>
@@ -3074,7 +3672,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>91</v>
       </c>
@@ -3094,7 +3692,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>91</v>
       </c>
@@ -3114,7 +3712,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>91</v>
       </c>
@@ -3134,7 +3732,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>91</v>
       </c>
@@ -3154,7 +3752,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>91</v>
       </c>
@@ -3174,7 +3772,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>92</v>
       </c>
@@ -3194,7 +3792,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>92</v>
       </c>
@@ -3214,7 +3812,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>92</v>
       </c>
@@ -3234,7 +3832,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>92</v>
       </c>
@@ -3254,7 +3852,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>92</v>
       </c>
@@ -3274,7 +3872,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>92</v>
       </c>
@@ -3294,7 +3892,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>92</v>
       </c>
@@ -3330,16 +3928,16 @@
   <dimension ref="B2:C24"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>54</v>
       </c>
@@ -3347,7 +3945,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>47</v>
       </c>
@@ -3355,7 +3953,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>49</v>
       </c>
@@ -3363,7 +3961,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>50</v>
       </c>
@@ -3371,7 +3969,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>38</v>
       </c>
@@ -3379,7 +3977,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>40</v>
       </c>
@@ -3387,7 +3985,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>48</v>
       </c>
@@ -3395,7 +3993,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>35</v>
       </c>
@@ -3403,7 +4001,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>42</v>
       </c>
@@ -3411,7 +4009,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>46</v>
       </c>
@@ -3419,7 +4017,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>45</v>
       </c>
@@ -3427,7 +4025,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>41</v>
       </c>
@@ -3435,7 +4033,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>36</v>
       </c>
@@ -3443,7 +4041,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>30</v>
       </c>
@@ -3451,7 +4049,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>51</v>
       </c>
@@ -3459,7 +4057,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>33</v>
       </c>
@@ -3467,7 +4065,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>34</v>
       </c>
@@ -3475,7 +4073,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>39</v>
       </c>
@@ -3483,7 +4081,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>32</v>
       </c>
@@ -3491,7 +4089,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>43</v>
       </c>
@@ -3499,7 +4097,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>44</v>
       </c>
@@ -3507,7 +4105,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>37</v>
       </c>
@@ -3515,7 +4113,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>31</v>
       </c>

</xml_diff>